<commit_message>
Updated this spreadsheet with events
</commit_message>
<xml_diff>
--- a/data/seminars.xlsx
+++ b/data/seminars.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20715" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725" iterate="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="583">
   <si>
     <t>date</t>
   </si>
@@ -1692,13 +1692,91 @@
   </si>
   <si>
     <t>https://numbersman77.github.io/kasparrufibach/files/talks/20231012_Rufibach_Lungevity_crossover.pdf</t>
+  </si>
+  <si>
+    <t>PSI Conference 2022</t>
+  </si>
+  <si>
+    <t>UPDATE - Estimand Implementation Working Group (EIWG)</t>
+  </si>
+  <si>
+    <t>EIWG-PSI-2022-Poster.pdf</t>
+  </si>
+  <si>
+    <t>01.11.2022</t>
+  </si>
+  <si>
+    <t>EFSPI Newsletter</t>
+  </si>
+  <si>
+    <t>How the Estimand Implementation Working Group brings together statisticians and clinicians to support the estimand journey</t>
+  </si>
+  <si>
+    <t>EIWG brings together statisticians and clinicians to support the estimand journey</t>
+  </si>
+  <si>
+    <t>13.09.2023</t>
+  </si>
+  <si>
+    <t>2022 PSI Annual Conference</t>
+  </si>
+  <si>
+    <t>Does the Estimand Framework Add Value to Clinical Pharmacology Trials?</t>
+  </si>
+  <si>
+    <t>Helle Lynggaard</t>
+  </si>
+  <si>
+    <t>Sue McKendrick</t>
+  </si>
+  <si>
+    <t>Amel Besseghir</t>
+  </si>
+  <si>
+    <t>Vivian Lanius</t>
+  </si>
+  <si>
+    <t>Christian Bressen Pipper</t>
+  </si>
+  <si>
+    <t>Khadija Rantell</t>
+  </si>
+  <si>
+    <t>Novo Nordisk</t>
+  </si>
+  <si>
+    <t>PPD Clinical Research Services</t>
+  </si>
+  <si>
+    <t>Thermo Fisher Scientific</t>
+  </si>
+  <si>
+    <t>UCB Pharma</t>
+  </si>
+  <si>
+    <t>MHRA</t>
+  </si>
+  <si>
+    <t>Leo Pharma</t>
+  </si>
+  <si>
+    <t>2024 EFSPI regulatory statistics workshop</t>
+  </si>
+  <si>
+    <t>Biozentrum Basel</t>
+  </si>
+  <si>
+    <t>11.09.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stefan Englert </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1737,6 +1815,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1759,7 +1843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1801,6 +1885,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1862,7 +1947,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1897,7 +1982,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2074,43 +2159,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="136.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.42578125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="84.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="84.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="72.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="13.86328125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="24.9296875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.06640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="10.53125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.59765625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="7.265625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="6.46484375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="6.1328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.53125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="21.86328125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="21.86328125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="14.53125" style="8" customWidth="1"/>
+    <col min="16" max="16" width="72.86328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2160,7 +2245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="12" t="str">
         <f>"15.02.2019"</f>
         <v>15.02.2019</v>
@@ -2199,7 +2284,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
@@ -2234,7 +2319,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -2257,7 +2342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2277,7 +2362,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -2297,7 +2382,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
@@ -2335,7 +2420,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -2355,7 +2440,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
@@ -2375,7 +2460,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
@@ -2395,7 +2480,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="8" t="s">
         <v>59</v>
       </c>
@@ -2430,7 +2515,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="8" t="s">
         <v>59</v>
       </c>
@@ -2450,7 +2535,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="28.5">
       <c r="A13" s="8" t="s">
         <v>64</v>
       </c>
@@ -2485,7 +2570,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="8" t="s">
         <v>72</v>
       </c>
@@ -2520,7 +2605,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="8" t="s">
         <v>80</v>
       </c>
@@ -2555,7 +2640,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="8" t="s">
         <v>80</v>
       </c>
@@ -2572,7 +2657,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="28.5">
       <c r="A17" s="8" t="s">
         <v>80</v>
       </c>
@@ -2589,7 +2674,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="8" t="s">
         <v>80</v>
       </c>
@@ -2606,7 +2691,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" s="8" t="s">
         <v>101</v>
       </c>
@@ -2644,7 +2729,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="8" t="s">
         <v>107</v>
       </c>
@@ -2676,7 +2761,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="8" t="s">
         <v>107</v>
       </c>
@@ -2693,7 +2778,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="8" t="s">
         <v>107</v>
       </c>
@@ -2713,7 +2798,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" s="8" t="s">
         <v>120</v>
       </c>
@@ -2745,7 +2830,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" s="8" t="s">
         <v>129</v>
       </c>
@@ -2777,7 +2862,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="A25" s="8" t="s">
         <v>135</v>
       </c>
@@ -2812,7 +2897,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="A26" s="8" t="s">
         <v>141</v>
       </c>
@@ -2847,7 +2932,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="A27" s="8" t="s">
         <v>141</v>
       </c>
@@ -2858,7 +2943,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16">
       <c r="A28" s="8" t="s">
         <v>148</v>
       </c>
@@ -2890,7 +2975,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="28.5">
       <c r="A29" s="8" t="s">
         <v>152</v>
       </c>
@@ -2931,7 +3016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" s="8" t="s">
         <v>152</v>
       </c>
@@ -2951,7 +3036,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16">
       <c r="A31" s="8" t="s">
         <v>152</v>
       </c>
@@ -2971,7 +3056,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16">
       <c r="A32" s="8" t="s">
         <v>152</v>
       </c>
@@ -2991,7 +3076,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="8" t="s">
         <v>152</v>
       </c>
@@ -3011,7 +3096,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="8" t="s">
         <v>152</v>
       </c>
@@ -3031,7 +3116,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="8" t="s">
         <v>152</v>
       </c>
@@ -3048,7 +3133,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="8" t="s">
         <v>180</v>
       </c>
@@ -3083,7 +3168,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="8" t="s">
         <v>180</v>
       </c>
@@ -3097,7 +3182,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="8" t="s">
         <v>185</v>
       </c>
@@ -3129,7 +3214,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="28.5">
       <c r="A39" s="8" t="s">
         <v>191</v>
       </c>
@@ -3170,7 +3255,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="8" t="s">
         <v>191</v>
       </c>
@@ -3190,7 +3275,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" s="8" t="s">
         <v>191</v>
       </c>
@@ -3210,7 +3295,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="28.5">
       <c r="A42" s="8" t="s">
         <v>191</v>
       </c>
@@ -3230,7 +3315,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" s="8" t="s">
         <v>191</v>
       </c>
@@ -3250,7 +3335,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" s="8" t="s">
         <v>191</v>
       </c>
@@ -3270,7 +3355,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="28.5">
       <c r="A45" s="8" t="s">
         <v>191</v>
       </c>
@@ -3290,7 +3375,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" s="8" t="s">
         <v>191</v>
       </c>
@@ -3310,7 +3395,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" s="8" t="s">
         <v>191</v>
       </c>
@@ -3330,7 +3415,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" s="8" t="s">
         <v>191</v>
       </c>
@@ -3347,7 +3432,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" s="8" t="s">
         <v>225</v>
       </c>
@@ -3382,7 +3467,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15">
       <c r="A50" s="8" t="s">
         <v>229</v>
       </c>
@@ -3417,7 +3502,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15">
       <c r="A51" s="8" t="s">
         <v>234</v>
       </c>
@@ -3455,7 +3540,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" s="8" t="s">
         <v>239</v>
       </c>
@@ -3493,7 +3578,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="A53" s="8" t="s">
         <v>244</v>
       </c>
@@ -3528,7 +3613,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="28.5">
       <c r="A54" s="8" t="s">
         <v>249</v>
       </c>
@@ -3563,7 +3648,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" s="8" t="s">
         <v>253</v>
       </c>
@@ -3595,7 +3680,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="42.75">
       <c r="A56" s="8" t="s">
         <v>257</v>
       </c>
@@ -3630,7 +3715,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="42.75">
       <c r="A57" s="8" t="s">
         <v>257</v>
       </c>
@@ -3647,7 +3732,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="42.75">
       <c r="A58" s="8" t="s">
         <v>257</v>
       </c>
@@ -3664,7 +3749,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="42.75">
       <c r="A59" s="8" t="s">
         <v>257</v>
       </c>
@@ -3681,7 +3766,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="42.75">
       <c r="A60" s="8" t="s">
         <v>257</v>
       </c>
@@ -3698,7 +3783,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15">
       <c r="A61" s="8" t="s">
         <v>262</v>
       </c>
@@ -3733,7 +3818,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15">
       <c r="A62" s="8" t="s">
         <v>262</v>
       </c>
@@ -3750,7 +3835,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" s="8" t="s">
         <v>262</v>
       </c>
@@ -3767,7 +3852,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" s="8" t="s">
         <v>262</v>
       </c>
@@ -3784,7 +3869,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15">
       <c r="A65" s="8" t="s">
         <v>262</v>
       </c>
@@ -3801,7 +3886,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15">
       <c r="A66" s="8" t="s">
         <v>262</v>
       </c>
@@ -3818,7 +3903,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15">
       <c r="A67" s="8" t="s">
         <v>271</v>
       </c>
@@ -3850,7 +3935,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="28.5">
       <c r="A68" s="8" t="s">
         <v>271</v>
       </c>
@@ -3864,7 +3949,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15">
       <c r="A69" s="8" t="s">
         <v>271</v>
       </c>
@@ -3881,7 +3966,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="28.5">
       <c r="A70" s="8" t="s">
         <v>271</v>
       </c>
@@ -3898,7 +3983,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="28.5">
       <c r="A71" s="8" t="str">
         <f>"24.08.2021"</f>
         <v>24.08.2021</v>
@@ -3934,7 +4019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15">
       <c r="A72" s="8" t="s">
         <v>279</v>
       </c>
@@ -3969,7 +4054,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15">
       <c r="A73" s="8" t="s">
         <v>279</v>
       </c>
@@ -3998,7 +4083,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15">
       <c r="A74" s="8" t="s">
         <v>279</v>
       </c>
@@ -4027,7 +4112,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15">
       <c r="A75" s="8" t="s">
         <v>279</v>
       </c>
@@ -4056,7 +4141,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15">
       <c r="A76" s="8" t="s">
         <v>279</v>
       </c>
@@ -4088,7 +4173,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15">
       <c r="A77" s="8" t="s">
         <v>289</v>
       </c>
@@ -4123,7 +4208,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15">
       <c r="A78" s="8" t="s">
         <v>289</v>
       </c>
@@ -4140,7 +4225,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15">
       <c r="A79" s="8" t="s">
         <v>289</v>
       </c>
@@ -4157,7 +4242,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15">
       <c r="A80" s="8" t="s">
         <v>289</v>
       </c>
@@ -4174,7 +4259,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15">
       <c r="A81" s="8" t="s">
         <v>289</v>
       </c>
@@ -4191,7 +4276,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15">
       <c r="A82" s="8" t="s">
         <v>289</v>
       </c>
@@ -4208,7 +4293,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="28.5">
       <c r="A83" s="8" t="s">
         <v>291</v>
       </c>
@@ -4240,7 +4325,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15">
       <c r="A84" s="8" t="s">
         <v>291</v>
       </c>
@@ -4257,7 +4342,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15">
       <c r="A85" s="8" t="str">
         <f>"16.12.2021"</f>
         <v>16.12.2021</v>
@@ -4293,7 +4378,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15">
       <c r="A86" s="8" t="str">
         <f>"23.03.2022"</f>
         <v>23.03.2022</v>
@@ -4329,7 +4414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15">
       <c r="A87" s="8" t="s">
         <v>296</v>
       </c>
@@ -4364,7 +4449,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="28.5">
       <c r="A88" s="8" t="s">
         <v>299</v>
       </c>
@@ -4396,7 +4481,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15">
       <c r="A89" s="8" t="s">
         <v>299</v>
       </c>
@@ -4413,7 +4498,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="28.5">
       <c r="A90" s="8" t="s">
         <v>302</v>
       </c>
@@ -4445,7 +4530,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15">
       <c r="A91" s="8" t="s">
         <v>307</v>
       </c>
@@ -4477,7 +4562,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15">
       <c r="A92" s="8" t="s">
         <v>307</v>
       </c>
@@ -4495,7 +4580,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15">
       <c r="A93" s="8" t="s">
         <v>307</v>
       </c>
@@ -4513,7 +4598,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="27">
       <c r="A94" s="8" t="s">
         <v>307</v>
       </c>
@@ -4531,7 +4616,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15">
       <c r="A95" s="8" t="s">
         <v>307</v>
       </c>
@@ -4549,7 +4634,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15">
       <c r="A96" s="8" t="s">
         <v>307</v>
       </c>
@@ -4567,7 +4652,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="28.5">
       <c r="A97" s="8" t="s">
         <v>313</v>
       </c>
@@ -4599,7 +4684,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15">
       <c r="A98" s="8" t="s">
         <v>320</v>
       </c>
@@ -4631,7 +4716,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15">
       <c r="A99" s="8" t="s">
         <v>326</v>
       </c>
@@ -4660,7 +4745,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15">
       <c r="A100" s="8" t="s">
         <v>330</v>
       </c>
@@ -4692,7 +4777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="28.5">
       <c r="A101" s="8" t="s">
         <v>334</v>
       </c>
@@ -4724,7 +4809,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15">
       <c r="A102" s="8" t="s">
         <v>340</v>
       </c>
@@ -4762,7 +4847,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15">
       <c r="A103" s="8" t="s">
         <v>342</v>
       </c>
@@ -4800,7 +4885,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15">
       <c r="A104" s="8" t="s">
         <v>342</v>
       </c>
@@ -4820,7 +4905,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15">
       <c r="A105" s="8" t="s">
         <v>342</v>
       </c>
@@ -4840,7 +4925,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="27">
       <c r="A106" s="8" t="s">
         <v>342</v>
       </c>
@@ -4858,7 +4943,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="28.5">
       <c r="A107" s="8" t="s">
         <v>346</v>
       </c>
@@ -4890,7 +4975,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15">
       <c r="A108" s="8" t="s">
         <v>351</v>
       </c>
@@ -4925,7 +5010,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="28.5">
       <c r="A109" s="8" t="s">
         <v>357</v>
       </c>
@@ -4963,7 +5048,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="27">
       <c r="A110" s="8" t="s">
         <v>357</v>
       </c>
@@ -4983,7 +5068,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="27">
       <c r="A111" s="8" t="s">
         <v>357</v>
       </c>
@@ -5003,7 +5088,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="27">
       <c r="A112" s="8" t="s">
         <v>357</v>
       </c>
@@ -5023,7 +5108,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" ht="27">
       <c r="A113" s="8" t="s">
         <v>357</v>
       </c>
@@ -5043,7 +5128,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16">
       <c r="A114" s="8" t="str">
         <f>"29.03.2023"</f>
         <v>29.03.2023</v>
@@ -5076,7 +5161,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16">
       <c r="A115" s="8" t="str">
         <f>"12.04.2023"</f>
         <v>12.04.2023</v>
@@ -5121,7 +5206,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" ht="28.5">
       <c r="A116" s="8" t="str">
         <f>"12.04.2023"</f>
         <v>12.04.2023</v>
@@ -5142,7 +5227,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16">
       <c r="A117" s="8" t="str">
         <f>"12.04.2023"</f>
         <v>12.04.2023</v>
@@ -5160,7 +5245,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16">
       <c r="A118" s="8" t="str">
         <f>"12.04.2023"</f>
         <v>12.04.2023</v>
@@ -5181,7 +5266,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16">
       <c r="A119" s="8" t="str">
         <f t="shared" ref="A119:A126" si="0">"31.05.2023"</f>
         <v>31.05.2023</v>
@@ -5220,7 +5305,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16">
       <c r="A120" s="8" t="str">
         <f t="shared" si="0"/>
         <v>31.05.2023</v>
@@ -5239,7 +5324,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" ht="28.5">
       <c r="A121" s="8" t="str">
         <f t="shared" si="0"/>
         <v>31.05.2023</v>
@@ -5261,7 +5346,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16">
       <c r="A122" s="8" t="str">
         <f t="shared" si="0"/>
         <v>31.05.2023</v>
@@ -5280,7 +5365,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" ht="28.5">
       <c r="A123" s="8" t="str">
         <f t="shared" si="0"/>
         <v>31.05.2023</v>
@@ -5302,7 +5387,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16">
       <c r="A124" s="8" t="str">
         <f t="shared" si="0"/>
         <v>31.05.2023</v>
@@ -5324,7 +5409,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16">
       <c r="A125" s="8" t="str">
         <f t="shared" si="0"/>
         <v>31.05.2023</v>
@@ -5346,7 +5431,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16">
       <c r="A126" s="8" t="str">
         <f t="shared" si="0"/>
         <v>31.05.2023</v>
@@ -5368,7 +5453,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16">
       <c r="A127" s="8" t="str">
         <f t="shared" ref="A127:A132" si="1">"11.06.2023"</f>
         <v>11.06.2023</v>
@@ -5407,7 +5492,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16">
       <c r="A128" s="8" t="str">
         <f t="shared" si="1"/>
         <v>11.06.2023</v>
@@ -5428,7 +5513,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16">
       <c r="A129" s="8" t="str">
         <f t="shared" si="1"/>
         <v>11.06.2023</v>
@@ -5443,7 +5528,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16">
       <c r="A130" s="8" t="str">
         <f t="shared" si="1"/>
         <v>11.06.2023</v>
@@ -5458,7 +5543,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16">
       <c r="A131" s="8" t="str">
         <f t="shared" si="1"/>
         <v>11.06.2023</v>
@@ -5479,7 +5564,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" ht="28.5">
       <c r="A132" s="8" t="str">
         <f t="shared" si="1"/>
         <v>11.06.2023</v>
@@ -5500,7 +5585,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16">
       <c r="A133" s="8" t="str">
         <f>"05.08.2023"</f>
         <v>05.08.2023</v>
@@ -5539,7 +5624,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" ht="28.5">
       <c r="A134" s="8" t="str">
         <f>"13.09.2023"</f>
         <v>13.09.2023</v>
@@ -5578,7 +5663,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16">
       <c r="A135" s="8" t="str">
         <f t="shared" ref="A135:A140" si="2">"29.09.2023"</f>
         <v>29.09.2023</v>
@@ -5617,7 +5702,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16">
       <c r="A136" s="8" t="str">
         <f t="shared" si="2"/>
         <v>29.09.2023</v>
@@ -5639,7 +5724,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16">
       <c r="A137" s="8" t="str">
         <f t="shared" si="2"/>
         <v>29.09.2023</v>
@@ -5661,7 +5746,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16">
       <c r="A138" s="8" t="str">
         <f t="shared" si="2"/>
         <v>29.09.2023</v>
@@ -5683,7 +5768,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16">
       <c r="A139" s="8" t="str">
         <f t="shared" si="2"/>
         <v>29.09.2023</v>
@@ -5705,7 +5790,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16">
       <c r="A140" s="8" t="str">
         <f t="shared" si="2"/>
         <v>29.09.2023</v>
@@ -5724,7 +5809,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16">
       <c r="A141" s="8" t="str">
         <f>"12.10.2023"</f>
         <v>12.10.2023</v>
@@ -5763,7 +5848,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" ht="42.75">
       <c r="A142" s="12" t="str">
         <f t="shared" ref="A142:A147" si="3">"16.10.2023"</f>
         <v>16.10.2023</v>
@@ -5799,7 +5884,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16">
       <c r="A143" s="12" t="str">
         <f t="shared" si="3"/>
         <v>16.10.2023</v>
@@ -5818,7 +5903,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16">
       <c r="A144" s="12" t="str">
         <f t="shared" si="3"/>
         <v>16.10.2023</v>
@@ -5837,7 +5922,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15">
       <c r="A145" s="12" t="str">
         <f t="shared" si="3"/>
         <v>16.10.2023</v>
@@ -5856,7 +5941,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15">
       <c r="A146" s="12" t="str">
         <f t="shared" si="3"/>
         <v>16.10.2023</v>
@@ -5875,7 +5960,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15">
       <c r="A147" s="12" t="str">
         <f t="shared" si="3"/>
         <v>16.10.2023</v>
@@ -5894,7 +5979,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15">
       <c r="A148" s="12" t="str">
         <f>"08.11.2023"</f>
         <v>08.11.2023</v>
@@ -5933,7 +6018,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="28.5">
       <c r="A149" s="8" t="str">
         <f>"24.11.2023"</f>
         <v>24.11.2023</v>
@@ -5969,7 +6054,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15">
       <c r="A150" s="8" t="str">
         <f>"24.11.2023"</f>
         <v>24.11.2023</v>
@@ -5994,7 +6079,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15">
       <c r="A151" s="8" t="str">
         <f>"16.06.2024"</f>
         <v>16.06.2024</v>
@@ -6014,9 +6099,231 @@
       <c r="F151" s="8" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M154"/>
+      <c r="O151" s="15"/>
+    </row>
+    <row r="152" spans="1:15">
+      <c r="A152" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="D152" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E152" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F152" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="G152" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K152" s="8">
+        <v>1</v>
+      </c>
+      <c r="L152" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="M152" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="N152" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="O152" s="8" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" ht="57">
+      <c r="A153" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="K153" s="8">
+        <v>1</v>
+      </c>
+      <c r="L153" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="M153" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="N153" s="9" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" ht="85.5">
+      <c r="A154" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="K154" s="8">
+        <v>1</v>
+      </c>
+      <c r="L154" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="M154" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="N154" s="9" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" ht="57">
+      <c r="A155" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="D155" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E155" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F155" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="G155" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K155" s="8">
+        <v>1</v>
+      </c>
+      <c r="L155" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="M155" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="N155" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="O155" s="8" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15">
+      <c r="K156" s="8">
+        <v>2</v>
+      </c>
+      <c r="L156" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="M156" s="8" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15">
+      <c r="K157" s="8">
+        <v>3</v>
+      </c>
+      <c r="L157" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="M157" s="8" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15">
+      <c r="K158" s="8">
+        <v>4</v>
+      </c>
+      <c r="L158" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="M158" s="8" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15">
+      <c r="K159" s="8">
+        <v>5</v>
+      </c>
+      <c r="L159" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="M159" s="8" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15">
+      <c r="K160" s="8">
+        <v>6</v>
+      </c>
+      <c r="L160" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="M160" s="8" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13">
+      <c r="K161" s="8">
+        <v>7</v>
+      </c>
+      <c r="L161" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="M161" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="28.5">
+      <c r="A162" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="E162" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F162" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="G162" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K162" s="8">
+        <v>1</v>
+      </c>
+      <c r="L162" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="M162" s="8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13">
+      <c r="K163" s="8">
+        <v>2</v>
+      </c>
+      <c r="L163" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="M163" s="8" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13">
+      <c r="K164" s="8">
+        <v>3</v>
+      </c>
+      <c r="L164" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="M164" s="8" t="s">
+        <v>577</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:P154">

</xml_diff>

<commit_message>
CHT fixes slide links 06 Aug 2024
</commit_message>
<xml_diff>
--- a/data/seminars.xlsx
+++ b/data/seminars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="103">
   <si>
     <t>date</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>12.06.23_13.30-15.00_1_ICH E9(R1)_impacts_beyond_Bioequivalence_Sue_Helle (1).pdf</t>
+  </si>
+  <si>
+    <t>EIWG_Clinical_Pharmacology_PSI_poster_02June2022_handout.pdf</t>
   </si>
 </sst>
 </file>
@@ -681,8 +684,8 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L22" sqref="L22:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -815,6 +818,12 @@
       <c r="D4" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>64</v>
       </c>
@@ -898,7 +907,7 @@
         <v>44</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1209,10 +1218,10 @@
         <v>1</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>99</v>
@@ -1245,10 +1254,10 @@
         <v>4</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:15">

</xml_diff>

<commit_message>
CHT 06 Aug 2024 fixed seminars spreadsheet
</commit_message>
<xml_diff>
--- a/data/seminars.xlsx
+++ b/data/seminars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="101">
   <si>
     <t>date</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Netherlands</t>
   </si>
   <si>
-    <t>PSI Conference 2022</t>
-  </si>
-  <si>
     <t>UPDATE - Estimand Implementation Working Group (EIWG)</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>2021 PSI Annual Conference</t>
   </si>
   <si>
-    <t>online</t>
-  </si>
-  <si>
     <t>Oral presentation</t>
   </si>
   <si>
@@ -324,10 +318,10 @@
     <t>Does it Make Sense to Apply the Estimand Framework to Clinical Pharmacology Trials?</t>
   </si>
   <si>
-    <t>12.06.23_13.30-15.00_1_ICH E9(R1)_impacts_beyond_Bioequivalence_Sue_Helle (1).pdf</t>
-  </si>
-  <si>
     <t>EIWG_Clinical_Pharmacology_PSI_poster_02June2022_handout.pdf</t>
+  </si>
+  <si>
+    <t>12.06.23_13.30-15.00_1_ICH E9(R1)_impacts_beyond_Bioequivalence_Sue_Helle.pdf</t>
   </si>
 </sst>
 </file>
@@ -673,7 +667,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -681,11 +675,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L22" sqref="L22:M22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -764,10 +758,10 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>26</v>
@@ -791,10 +785,10 @@
         <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -802,142 +796,97 @@
         <v>2</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="57">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>65</v>
+      <c r="L4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="85.5">
-      <c r="A5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="57">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="K6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="K7" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="K8" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="K9" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>54</v>
@@ -945,46 +894,91 @@
     </row>
     <row r="10" spans="1:16">
       <c r="K10" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="57">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="K11" s="1">
-        <v>6</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="85.5">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K12" s="1">
-        <v>7</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="57">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>21</v>
@@ -999,13 +993,13 @@
         <v>1</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1013,10 +1007,10 @@
         <v>2</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1024,42 +1018,45 @@
         <v>3</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="42.75">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K16" s="1">
         <v>1</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="O16" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1067,45 +1064,45 @@
         <v>2</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="42.75">
       <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K18" s="1">
         <v>1</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="42.75">
@@ -1113,94 +1110,70 @@
         <v>1</v>
       </c>
       <c r="L19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="28.5">
+    </row>
+    <row r="20" spans="1:15" ht="57">
       <c r="A20" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K20" s="1">
         <v>1</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="K21" s="1">
+        <v>2</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="42.75">
-      <c r="A21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K21" s="1">
-        <v>1</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="71.25">
+    </row>
+    <row r="22" spans="1:15" ht="28.5">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>33</v>
@@ -1212,24 +1185,45 @@
         <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="K22" s="1">
         <v>1</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+        <v>88</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="42.75">
+      <c r="A23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="K23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>32</v>
@@ -1237,96 +1231,107 @@
       <c r="M23" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="N23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="71.25">
+      <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="K24" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>16</v>
+      <c r="N24" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="K25" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="K26" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="K27" s="1">
+        <v>4</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="K28" s="1">
+        <v>5</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="K29" s="1">
         <v>6</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K28" s="1">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="57">
-      <c r="K29" s="1">
-        <v>2</v>
-      </c>
       <c r="L29" s="1" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="B30" s="1"/>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="B31" s="1"/>
+      <c r="N31" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:P154">

</xml_diff>